<commit_message>
Added event summary for the Missing Sheeps
</commit_message>
<xml_diff>
--- a/Stories/MissingSheep.xlsx
+++ b/Stories/MissingSheep.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\DECO3801-Synergistiscs\Stories\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School Related\DECO3801\DECO3801-Synergistiscs\Stories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55CDB513-9A6F-451A-8C3E-EAB615FA1AEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E1E35E-758C-488D-8C72-0FB3B487F98B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="100">
   <si>
     <t>MILITARY</t>
   </si>
@@ -296,6 +296,36 @@
   </si>
   <si>
     <t>FARM</t>
+  </si>
+  <si>
+    <t>EVENT SUMMARY HEADER</t>
+  </si>
+  <si>
+    <t>ACTION 1 EVENT SUMMARY</t>
+  </si>
+  <si>
+    <t>ACTION 2 EVENT SUMMARY</t>
+  </si>
+  <si>
+    <t>ACTION 3 EVENT SUMMARY</t>
+  </si>
+  <si>
+    <t>ACTION 4 EVENT SUMMARY</t>
+  </si>
+  <si>
+    <t>While you were focused on handling these minor affairs in your Kingdom, the disease that is currently affecting the neighbouring Kingdoms have starting to take effect within your own Kingdom.</t>
+  </si>
+  <si>
+    <t>Having to allocate military personnel to such matters meant that you were lacking manpower to support the efforts in trying to maintain and contain the disease.</t>
+  </si>
+  <si>
+    <t>Your decision to ignore this issue had caused it to escalate into riots and fighting between these farmers. This had also further accelerated the spread of the disease within the Kingdom.</t>
+  </si>
+  <si>
+    <t>By giving money to these farmers to quell the issue, you managed to settle this issue for now. However, it came at a cost of the Kingdom's treasury.</t>
+  </si>
+  <si>
+    <t>Although it had sparked some concerns with the villagers, this was a good move as you managed to get rid the source of this issue. This also meant that you had more time to focus on the disease spreading within the city.</t>
   </si>
 </sst>
 </file>
@@ -478,69 +508,69 @@
   </cellStyleXfs>
   <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -822,427 +852,532 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="17"/>
+      <c r="F1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="17"/>
+      <c r="H1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="1" t="s">
+      <c r="I1" s="17"/>
+      <c r="J1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="1" t="s">
+      <c r="K1" s="17"/>
+      <c r="L1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="2"/>
-    </row>
-    <row r="2" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7" t="s">
+      <c r="M1" s="17"/>
+    </row>
+    <row r="2" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="2"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="b">
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="17"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="2"/>
-    </row>
-    <row r="5" spans="1:13" ht="256.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="17"/>
+    </row>
+    <row r="5" spans="1:13" ht="248.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="2"/>
-    </row>
-    <row r="7" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="17"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="2"/>
-    </row>
-    <row r="8" spans="1:13" ht="199.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="17"/>
+    </row>
+    <row r="8" spans="1:13" ht="193.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K8" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="L8" s="11" t="s">
+      <c r="L8" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="M8" s="11" t="s">
+      <c r="M8" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="1:13" ht="213.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="17"/>
+    </row>
+    <row r="10" spans="1:13" ht="207" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="I10" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="K10" s="10" t="s">
+      <c r="K10" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="L10" s="10" t="s">
+      <c r="L10" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="M10" s="10" t="s">
+      <c r="M10" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="2"/>
-    </row>
-    <row r="12" spans="1:13" ht="213.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="17"/>
+    </row>
+    <row r="12" spans="1:13" ht="207" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="I12" s="15" t="s">
+      <c r="I12" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="J12" s="15" t="s">
+      <c r="J12" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="K12" s="15" t="s">
+      <c r="K12" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="L12" s="15" t="s">
+      <c r="L12" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="M12" s="15" t="s">
+      <c r="M12" s="11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="2"/>
-    </row>
-    <row r="14" spans="1:13" ht="242.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="17"/>
+    </row>
+    <row r="14" spans="1:13" ht="248.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="I14" s="10" t="s">
+      <c r="I14" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J14" s="10" t="s">
+      <c r="J14" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="K14" s="10" t="s">
+      <c r="K14" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="L14" s="10" t="s">
+      <c r="L14" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="M14" s="10" t="s">
+      <c r="M14" s="6" t="s">
         <v>88</v>
       </c>
     </row>
+    <row r="15" spans="1:13" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="17"/>
+    </row>
+    <row r="16" spans="1:13" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="17"/>
+    </row>
+    <row r="17" spans="1:13" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="17"/>
+    </row>
+    <row r="18" spans="1:13" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="17"/>
+    </row>
+    <row r="19" spans="1:13" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="17"/>
+    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="18">
+    <mergeCell ref="B15:M15"/>
+    <mergeCell ref="B16:M16"/>
+    <mergeCell ref="B17:M17"/>
+    <mergeCell ref="B18:M18"/>
+    <mergeCell ref="B19:M19"/>
+    <mergeCell ref="B7:M7"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B11:M11"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="L1:M1"/>
     <mergeCell ref="B3:M3"/>
     <mergeCell ref="B4:M4"/>
     <mergeCell ref="B6:M6"/>
@@ -1251,11 +1386,6 @@
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
-    <mergeCell ref="B7:M7"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B11:M11"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="L1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Proof read and amendments to summary.
Proof read the summary outcomes for any grammatical errors and made amendements to have it suit the stories better.
</commit_message>
<xml_diff>
--- a/Stories/MissingSheep.xlsx
+++ b/Stories/MissingSheep.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School Related\DECO3801\DECO3801-Synergistiscs\Stories\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C2C5AC-A440-4501-9594-3C071B98C374}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="23257" windowHeight="12580"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -207,16 +213,10 @@
     <t>ACTION 4 EVENT SUMMARY</t>
   </si>
   <si>
-    <t>While you were focused on handling these minor affairs in your Kingdom, the disease that is currently affecting the neighbouring Kingdoms have starting to take effect within your own Kingdom.</t>
-  </si>
-  <si>
     <t>Having to allocate military personnel to such matters meant that you were lacking manpower to support the efforts in trying to maintain and contain the disease.</t>
   </si>
   <si>
     <t>Your decision to ignore this issue had caused it to escalate into riots and fighting between these farmers. This had also further accelerated the spread of the disease within the Kingdom.</t>
-  </si>
-  <si>
-    <t>By giving money to these farmers to quell the issue, you managed to settle this issue for now. However, it came at a cost of the Kingdom's treasury.</t>
   </si>
   <si>
     <t>Although it had sparked some concerns with the villagers, this was a good move as you managed to get rid the source of this issue. This also meant that you had more time to focus on the disease spreading within the city.</t>
@@ -320,12 +320,18 @@
   </si>
   <si>
     <t>I believe other neighbouring kingdoms do it this way as well.</t>
+  </si>
+  <si>
+    <t>While you were focused on handling these minor affairs in your Kingdom, the disease that is currently affecting the neighbouring Kingdoms have started to take effect within your own Kingdom.</t>
+  </si>
+  <si>
+    <t>By giving money to these farmers to quell the disturbance, you managed to resolve this matter for now. However, it came at a hugh cost of the Kingdom's treasury.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -561,93 +567,93 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -917,57 +923,57 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.125" customWidth="1"/>
-    <col min="4" max="4" width="14.625" customWidth="1"/>
-    <col min="5" max="5" width="14.875" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="20" t="s">
+      <c r="C1" s="40"/>
+      <c r="D1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="20" t="s">
+      <c r="E1" s="29"/>
+      <c r="F1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="20" t="s">
+      <c r="G1" s="29"/>
+      <c r="H1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="20" t="s">
+      <c r="I1" s="29"/>
+      <c r="J1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="23"/>
-      <c r="L1" s="20" t="s">
+      <c r="K1" s="29"/>
+      <c r="L1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="23"/>
-    </row>
-    <row r="2" spans="1:13" ht="27.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M1" s="29"/>
+    </row>
+    <row r="2" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>6</v>
@@ -1006,59 +1012,59 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="26"/>
-    </row>
-    <row r="4" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="32"/>
+    </row>
+    <row r="4" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="B4" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="29"/>
-    </row>
-    <row r="5" spans="1:13" ht="256.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="35"/>
+    </row>
+    <row r="5" spans="1:13" ht="248.4" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="E5" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>71</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>20</v>
@@ -1066,8 +1072,8 @@
       <c r="G5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="31" t="s">
-        <v>72</v>
+      <c r="H5" s="16" t="s">
+        <v>70</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>22</v>
@@ -1078,52 +1084,52 @@
       <c r="K5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="31" t="s">
-        <v>73</v>
+      <c r="L5" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="M5" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="34"/>
-    </row>
-    <row r="7" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="38"/>
+    </row>
+    <row r="7" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="36"/>
-    </row>
-    <row r="8" spans="1:13" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="21"/>
+    </row>
+    <row r="8" spans="1:13" ht="193.2" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -1139,8 +1145,8 @@
       <c r="E8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="31" t="s">
-        <v>75</v>
+      <c r="F8" s="16" t="s">
+        <v>73</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>33</v>
@@ -1148,8 +1154,8 @@
       <c r="H8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="30" t="s">
-        <v>76</v>
+      <c r="I8" s="15" t="s">
+        <v>74</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>35</v>
@@ -1157,38 +1163,38 @@
       <c r="K8" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="L8" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="M8" s="30" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L8" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="38"/>
-    </row>
-    <row r="10" spans="1:13" ht="214" x14ac:dyDescent="0.25">
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="24"/>
+    </row>
+    <row r="10" spans="1:13" ht="207" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>39</v>
@@ -1206,52 +1212,52 @@
         <v>42</v>
       </c>
       <c r="H10" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="J10" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>82</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>43</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="40"/>
-      <c r="M11" s="41"/>
-    </row>
-    <row r="12" spans="1:13" ht="207" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="27"/>
+    </row>
+    <row r="12" spans="1:13" ht="207" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="42" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="43" t="s">
-        <v>87</v>
+      <c r="B12" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>85</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>45</v>
@@ -1266,55 +1272,55 @@
         <v>48</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I12" s="11" t="s">
         <v>49</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K12" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="L12" s="42" t="s">
-        <v>90</v>
-      </c>
-      <c r="M12" s="42" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L12" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="M12" s="17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="40"/>
-      <c r="L13" s="40"/>
-      <c r="M13" s="41"/>
-    </row>
-    <row r="14" spans="1:13" ht="242.5" x14ac:dyDescent="0.25">
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="27"/>
+    </row>
+    <row r="14" spans="1:13" ht="248.4" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>53</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>32</v>
@@ -1326,121 +1332,126 @@
         <v>55</v>
       </c>
       <c r="H14" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="J14" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="I14" s="31" t="s">
+      <c r="K14" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="J14" s="31" t="s">
+      <c r="L14" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="K14" s="6" t="s">
+      <c r="M14" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="L14" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="M14" s="31" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="42.8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:13" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="17"/>
-    </row>
-    <row r="16" spans="1:13" ht="41.45" x14ac:dyDescent="0.3">
+      <c r="B15" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="43"/>
+    </row>
+    <row r="16" spans="1:13" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="17"/>
-    </row>
-    <row r="17" spans="1:13" ht="41.45" x14ac:dyDescent="0.3">
+      <c r="B16" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="43"/>
+    </row>
+    <row r="17" spans="1:13" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="17"/>
-    </row>
-    <row r="18" spans="1:13" ht="41.45" x14ac:dyDescent="0.3">
+      <c r="B17" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="43"/>
+    </row>
+    <row r="18" spans="1:13" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="17"/>
-    </row>
-    <row r="19" spans="1:13" ht="41.45" x14ac:dyDescent="0.3">
+      <c r="B18" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="43"/>
+    </row>
+    <row r="19" spans="1:13" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="17"/>
+      <c r="B19" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="42"/>
+      <c r="M19" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B15:M15"/>
+    <mergeCell ref="B16:M16"/>
+    <mergeCell ref="B17:M17"/>
+    <mergeCell ref="B18:M18"/>
+    <mergeCell ref="B19:M19"/>
     <mergeCell ref="B7:M7"/>
     <mergeCell ref="B9:M9"/>
     <mergeCell ref="B11:M11"/>
@@ -1454,11 +1465,6 @@
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
-    <mergeCell ref="B15:M15"/>
-    <mergeCell ref="B16:M16"/>
-    <mergeCell ref="B17:M17"/>
-    <mergeCell ref="B18:M18"/>
-    <mergeCell ref="B19:M19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>